<commit_message>
arreglo error formato excel
</commit_message>
<xml_diff>
--- a/ApiGateway/ApiGatewayExpedientes/public/formato_personas (1) (1).xlsx.xlsx
+++ b/ApiGateway/ApiGatewayExpedientes/public/formato_personas (1) (1).xlsx.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652BF0F1-B09E-4280-A714-4770428DF8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B20CBA4-CB94-40E3-9195-D135EDBCCBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
   <si>
     <t>Nombres</t>
   </si>
@@ -53,17 +53,56 @@
     <t>correo@correo.com</t>
   </si>
   <si>
-    <t>321sda</t>
-  </si>
-  <si>
-    <t>fsd</t>
+    <t>Nombres 1</t>
+  </si>
+  <si>
+    <t>identificacion1</t>
+  </si>
+  <si>
+    <t>Nombres 2</t>
+  </si>
+  <si>
+    <t>identificacion2</t>
+  </si>
+  <si>
+    <t>Nombres 3</t>
+  </si>
+  <si>
+    <t>Nombres 4</t>
+  </si>
+  <si>
+    <t>Nombres 5</t>
+  </si>
+  <si>
+    <t>Nombres 6</t>
+  </si>
+  <si>
+    <t>Nombres 7</t>
+  </si>
+  <si>
+    <t>Nombres 8</t>
+  </si>
+  <si>
+    <t>Nombres 9</t>
+  </si>
+  <si>
+    <t>Nombres 10</t>
+  </si>
+  <si>
+    <t>Nombres 11</t>
+  </si>
+  <si>
+    <t>Nombres 12</t>
+  </si>
+  <si>
+    <t>identificacion3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +120,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,7 +187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -156,12 +203,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB7DEE8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB7DEE8"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -595,7 +657,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -624,13 +686,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1">
         <v>3002156987</v>
@@ -641,12 +703,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:E41">
-    <cfRule type="containsBlanks" dxfId="12" priority="2">
+    <cfRule type="containsBlanks" dxfId="14" priority="2">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:E2">
-    <cfRule type="containsBlanks" dxfId="11" priority="1">
+    <cfRule type="containsBlanks" dxfId="13" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -700,13 +762,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>32513521351</v>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="1">
         <v>3002156987</v>
@@ -720,13 +782,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <v>65654</v>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D3" s="1">
         <v>3002156987</v>
@@ -739,14 +801,19 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:E41">
-    <cfRule type="containsBlanks" dxfId="10" priority="1">
+  <conditionalFormatting sqref="A3:E41">
+    <cfRule type="containsBlanks" dxfId="12" priority="2">
+      <formula>LEN(TRIM(A3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:E2">
+    <cfRule type="containsBlanks" dxfId="11" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{2F63A68F-A320-49FD-8E9F-AD12ECB788B0}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{C3B2029A-F965-4983-9F6A-9182C4A01427}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{C3B2029A-F965-4983-9F6A-9182C4A01427}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{9A3FA456-B3E0-4305-9DD7-4552232E103F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
@@ -758,7 +825,7 @@
   <sheetPr>
     <tabColor rgb="FF5C9E31"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -768,11 +835,12 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="20.6328125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="15.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -789,15 +857,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>32551235</v>
+        <v>202215203458</v>
       </c>
       <c r="D2" s="1">
         <v>3002156987</v>
@@ -807,16 +875,16 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1">
         <f>C2+1</f>
-        <v>32551236</v>
+        <v>202215203459</v>
       </c>
       <c r="D3" s="1">
         <v>3002156987</v>
@@ -825,16 +893,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" ref="C4:C10" si="0">C3+1</f>
-        <v>32551237</v>
+        <v>202215203460</v>
       </c>
       <c r="D4" s="1">
         <v>3002156987</v>
@@ -843,16 +911,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>32551238</v>
+        <v>202215203461</v>
       </c>
       <c r="D5" s="1">
         <v>3002156987</v>
@@ -861,16 +929,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>32551239</v>
+        <v>202215203462</v>
       </c>
       <c r="D6" s="1">
         <v>3002156987</v>
@@ -879,16 +947,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>32551240</v>
+        <v>202215203463</v>
       </c>
       <c r="D7" s="1">
         <v>3002156987</v>
@@ -897,16 +965,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>32551241</v>
+        <v>202215203464</v>
       </c>
       <c r="D8" s="1">
         <v>3002156987</v>
@@ -915,16 +983,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>32551242</v>
+        <v>202215203465</v>
       </c>
       <c r="D9" s="1">
         <v>3002156987</v>
@@ -933,16 +1001,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>32551243</v>
+        <v>202215203466</v>
       </c>
       <c r="D10" s="1">
         <v>3002156987</v>
@@ -950,56 +1018,64 @@
       <c r="E10" s="6" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K14" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A11:E41">
+    <cfRule type="containsBlanks" dxfId="10" priority="12">
+      <formula>LEN(TRIM(A11))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:E2">
     <cfRule type="containsBlanks" dxfId="9" priority="11">
-      <formula>LEN(TRIM(A11))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:E2">
-    <cfRule type="containsBlanks" dxfId="8" priority="10">
+      <formula>LEN(TRIM(B2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:E3 C4:C10">
+    <cfRule type="containsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(A3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:B4 D4:E4">
+    <cfRule type="containsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(A4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:B5 D5:E5">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(A5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:B6 D6:E6">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(A6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:B7 D7:E7">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(A7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:B8 D8:E8">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A8))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:B9 D9:E9">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(A9))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:B10 D10:E10">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(A10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:E3 C4:C10">
-    <cfRule type="containsBlanks" dxfId="7" priority="8">
-      <formula>LEN(TRIM(A3))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4:B4 D4:E4">
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
-      <formula>LEN(TRIM(A4))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5:B5 D5:E5">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(A5))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A6:B6 D6:E6">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(A6))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7:B7 D7:E7">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(A7))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8:B8 D8:E8">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(A8))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9:B9 D9:E9">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(A9))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10:B10 D10:E10">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -1014,6 +1090,6 @@
     <hyperlink ref="E10" r:id="rId9" xr:uid="{FADE277C-170F-4D77-A8C0-F802F7D86D6C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>